<commit_message>
updated userstories and meeting protocol doc
</commit_message>
<xml_diff>
--- a/doc/project_documentation/UserStories.xlsx
+++ b/doc/project_documentation/UserStories.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aauklagenfurt-my.sharepoint.com/personal/andrkogler_edu_aau_at/Documents/SE2-Gruppe2_MovingMaze/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Skryy\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="11_92483E2D04E89AD36523F29B863E8C1851038389" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FC62FBF-E9AB-4AAD-AEC3-13035D27D821}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F76DC78-ACCD-4110-9628-19BEFA37E697}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6440" yWindow="460" windowWidth="22360" windowHeight="15360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Gamboard" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
   <si>
     <t>Feature</t>
   </si>
@@ -182,13 +182,19 @@
   </si>
   <si>
     <t>Spielbrett Inizaliseiren</t>
+  </si>
+  <si>
+    <t>Loading Screen</t>
+  </si>
+  <si>
+    <t>Beim Start des Spiels sollte ein Ladescreen erscheinen der mich (zB mittels progressbar) darüber informiert wie weit das Spiel bereits geladen ist.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,7 +264,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -554,13 +560,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView zoomScale="116" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.28515625" customWidth="1"/>
     <col min="2" max="2" width="38.42578125" customWidth="1"/>
@@ -569,7 +575,7 @@
     <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -586,7 +592,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="32.1">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -600,7 +606,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -614,7 +620,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -628,7 +634,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -642,7 +648,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="60">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -656,7 +662,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="45">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -667,7 +673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -678,7 +684,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -692,7 +698,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -706,7 +712,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -720,7 +726,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -731,7 +737,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -745,7 +751,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -756,7 +762,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -767,7 +773,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -778,7 +784,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -789,8 +795,23 @@
         <v>41</v>
       </c>
     </row>
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -798,32 +819,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47501C7-6ACF-4E88-AF07-41A7C2069411}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>

</xml_diff>